<commit_message>
match time and time zone
fix issues for common time zones, ordered data best third teams according to date and match time
</commit_message>
<xml_diff>
--- a/data/out/wiki/men/uefa/wc/goals_wc_uefa_men.xlsx
+++ b/data/out/wiki/men/uefa/wc/goals_wc_uefa_men.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -573,7 +573,7 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['Italy', 'Bulgaria', 'Argentina']</t>
+          <t>['Argentina', 'Italy', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -653,7 +653,7 @@
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
-          <t>['Italy', 'Bulgaria', 'Argentina']</t>
+          <t>['Argentina', 'Italy', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>['Italy', 'Bulgaria', 'Argentina']</t>
+          <t>['Argentina', 'Italy', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -829,7 +829,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>['Italy', 'Bulgaria', 'Argentina']</t>
+          <t>['Argentina', 'Italy', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -917,7 +917,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>['Italy', 'Bulgaria', 'Argentina']</t>
+          <t>['Argentina', 'Italy', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>['Italy', 'Bulgaria', 'Argentina']</t>
+          <t>['Argentina', 'Italy', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>['Italy', 'Bulgaria', 'Argentina']</t>
+          <t>['Argentina', 'Italy', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>['Italy', 'Bulgaria', 'Argentina']</t>
+          <t>['Argentina', 'Italy', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1269,7 +1269,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>['Italy', 'Bulgaria', 'Argentina']</t>
+          <t>['Argentina', 'Italy', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1343,7 +1343,7 @@
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr">
         <is>
-          <t>['Mexico', 'Belgium', 'Paraguay']</t>
+          <t>['Paraguay', 'Mexico', 'Belgium']</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1423,7 +1423,7 @@
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr">
         <is>
-          <t>['Mexico', 'Belgium', 'Paraguay']</t>
+          <t>['Paraguay', 'Mexico', 'Belgium']</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1511,7 +1511,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>['Mexico', 'Belgium', 'Paraguay']</t>
+          <t>['Paraguay', 'Mexico', 'Belgium']</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1599,7 +1599,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>['Mexico', 'Belgium', 'Paraguay']</t>
+          <t>['Paraguay', 'Mexico', 'Belgium']</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1687,7 +1687,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>['Mexico', 'Belgium', 'Paraguay']</t>
+          <t>['Paraguay', 'Mexico', 'Belgium']</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1775,7 +1775,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>['Mexico', 'Belgium', 'Paraguay']</t>
+          <t>['Paraguay', 'Mexico', 'Belgium']</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1863,7 +1863,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>['Mexico', 'Belgium', 'Paraguay']</t>
+          <t>['Paraguay', 'Mexico', 'Belgium']</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1937,7 +1937,7 @@
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr">
         <is>
-          <t>['Hungary', 'France', 'Soviet Union']</t>
+          <t>['France', 'Soviet Union', 'Hungary']</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -2017,7 +2017,7 @@
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
         <is>
-          <t>['Hungary', 'France', 'Soviet Union']</t>
+          <t>['France', 'Soviet Union', 'Hungary']</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -2105,7 +2105,7 @@
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr">
         <is>
-          <t>['Hungary', 'France', 'Soviet Union']</t>
+          <t>['France', 'Soviet Union', 'Hungary']</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -2197,7 +2197,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Hungary', 'France']</t>
+          <t>['Soviet Union', 'France', 'Hungary']</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -2223,18 +2223,18 @@
       </c>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>['France', 'Soviet Union', 'Hungary']</t>
+          <t>['France', 'Soviet Union']</t>
         </is>
       </c>
       <c r="S21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U21" t="n">
         <v>1892</v>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>['Hungary', 'France', 'Soviet Union']</t>
+          <t>['France', 'Soviet Union', 'Hungary']</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2311,18 +2311,18 @@
       </c>
       <c r="P22" t="inlineStr"/>
       <c r="Q22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'France', 'Hungary']</t>
+          <t>['Soviet Union', 'France']</t>
         </is>
       </c>
       <c r="S22" t="n">
         <v>0</v>
       </c>
       <c r="T22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U22" t="n">
         <v>1942</v>
@@ -2373,7 +2373,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>['Hungary', 'France', 'Soviet Union']</t>
+          <t>['France', 'Soviet Union', 'Hungary']</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2407,7 +2407,7 @@
         </is>
       </c>
       <c r="S23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T23" t="n">
         <v>1</v>
@@ -2461,7 +2461,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>['Hungary', 'France', 'Soviet Union']</t>
+          <t>['France', 'Soviet Union', 'Hungary']</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2549,7 +2549,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>['Hungary', 'France', 'Soviet Union']</t>
+          <t>['France', 'Soviet Union', 'Hungary']</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2623,7 +2623,7 @@
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
-          <t>['Brazil', 'Spain', 'Northern Ireland']</t>
+          <t>['Spain', 'Northern Ireland', 'Brazil']</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2703,7 +2703,7 @@
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr">
         <is>
-          <t>['Brazil', 'Spain', 'Northern Ireland']</t>
+          <t>['Spain', 'Northern Ireland', 'Brazil']</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2787,7 +2787,7 @@
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr">
         <is>
-          <t>['Brazil', 'Spain', 'Northern Ireland']</t>
+          <t>['Spain', 'Northern Ireland', 'Brazil']</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2875,7 +2875,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>['Brazil', 'Algeria', 'Spain']</t>
+          <t>['Spain', 'Algeria', 'Brazil']</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2963,7 +2963,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>['Brazil', 'Spain', 'Northern Ireland']</t>
+          <t>['Spain', 'Northern Ireland', 'Brazil']</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -3051,7 +3051,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>['Brazil', 'Algeria', 'Spain']</t>
+          <t>['Spain', 'Algeria', 'Brazil']</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -3139,7 +3139,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>['Brazil', 'Spain', 'Northern Ireland']</t>
+          <t>['Spain', 'Northern Ireland', 'Brazil']</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -3227,7 +3227,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>['Brazil', 'Spain', 'Northern Ireland']</t>
+          <t>['Spain', 'Northern Ireland', 'Brazil']</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -3315,7 +3315,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>['Brazil', 'Spain', 'Northern Ireland']</t>
+          <t>['Spain', 'Northern Ireland', 'Brazil']</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -3389,7 +3389,7 @@
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr">
         <is>
-          <t>['Denmark', 'West Germany', 'Uruguay']</t>
+          <t>['Denmark', 'Uruguay', 'West Germany']</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3469,7 +3469,7 @@
       <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr">
         <is>
-          <t>['Denmark', 'West Germany', 'Uruguay']</t>
+          <t>['Denmark', 'Uruguay', 'West Germany']</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3553,7 +3553,7 @@
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr">
         <is>
-          <t>['Denmark', 'West Germany', 'Uruguay']</t>
+          <t>['Denmark', 'Uruguay', 'West Germany']</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3641,7 +3641,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>['Denmark', 'West Germany', 'Uruguay']</t>
+          <t>['Denmark', 'Uruguay', 'West Germany']</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3667,18 +3667,18 @@
       </c>
       <c r="P38" t="inlineStr"/>
       <c r="Q38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R38" t="inlineStr">
         <is>
-          <t>['Denmark', 'West Germany']</t>
+          <t>['Denmark', 'West Germany', 'Uruguay']</t>
         </is>
       </c>
       <c r="S38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U38" t="n">
         <v>1892</v>
@@ -3729,7 +3729,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>['Denmark', 'West Germany', 'Uruguay']</t>
+          <t>['Denmark', 'Uruguay', 'West Germany']</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3755,18 +3755,18 @@
       </c>
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>['Denmark', 'West Germany', 'Uruguay']</t>
+          <t>['Denmark', 'West Germany']</t>
         </is>
       </c>
       <c r="S39" t="n">
         <v>1</v>
       </c>
       <c r="T39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U39" t="n">
         <v>1892</v>
@@ -3803,7 +3803,7 @@
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr">
         <is>
-          <t>['Morocco', 'Poland', 'Portugal']</t>
+          <t>['Poland', 'Portugal', 'Morocco']</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3883,7 +3883,7 @@
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr">
         <is>
-          <t>['Morocco', 'Poland', 'Portugal']</t>
+          <t>['Poland', 'Portugal', 'Morocco']</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3971,7 +3971,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>['England', 'Poland', 'Portugal']</t>
+          <t>['Poland', 'Portugal', 'England']</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -4059,7 +4059,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>['England', 'Morocco', 'Portugal']</t>
+          <t>['Portugal', 'Morocco', 'England']</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -4147,7 +4147,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>['England', 'Morocco', 'Poland']</t>
+          <t>['Poland', 'Morocco', 'England']</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -4235,7 +4235,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>['England', 'Morocco', 'Poland']</t>
+          <t>['Poland', 'Morocco', 'England']</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -4323,7 +4323,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>['England', 'Morocco', 'Poland']</t>
+          <t>['Poland', 'Morocco', 'England']</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -4411,7 +4411,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>['England', 'Morocco', 'Poland']</t>
+          <t>['Poland', 'Morocco', 'England']</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -4499,7 +4499,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>['England', 'Morocco', 'Poland']</t>
+          <t>['Poland', 'Morocco', 'England']</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -4573,7 +4573,7 @@
       <c r="I49" t="inlineStr"/>
       <c r="J49" t="inlineStr">
         <is>
-          <t>['Austria', 'Czechoslovakia', 'Italy']</t>
+          <t>['Czechoslovakia', 'Italy', 'Austria']</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -4657,7 +4657,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>['Austria', 'Czechoslovakia', 'Italy']</t>
+          <t>['Czechoslovakia', 'Italy', 'Austria']</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -4745,7 +4745,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>['Austria', 'Czechoslovakia', 'Italy']</t>
+          <t>['Czechoslovakia', 'Italy', 'Austria']</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4833,7 +4833,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>['Austria', 'Czechoslovakia', 'Italy']</t>
+          <t>['Czechoslovakia', 'Italy', 'Austria']</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4921,7 +4921,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>['Austria', 'Czechoslovakia', 'Italy']</t>
+          <t>['Czechoslovakia', 'Italy', 'Austria']</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4947,18 +4947,18 @@
       </c>
       <c r="P53" t="inlineStr"/>
       <c r="Q53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R53" t="inlineStr">
         <is>
-          <t>['Italy', 'Czechoslovakia']</t>
+          <t>['Italy', 'Czechoslovakia', 'Austria']</t>
         </is>
       </c>
       <c r="S53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U53" t="n">
         <v>1966</v>
@@ -5009,7 +5009,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>['Austria', 'Czechoslovakia', 'Italy']</t>
+          <t>['Czechoslovakia', 'Italy', 'Austria']</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -5035,18 +5035,18 @@
       </c>
       <c r="P54" t="inlineStr"/>
       <c r="Q54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R54" t="inlineStr">
         <is>
-          <t>['Italy', 'Czechoslovakia', 'Austria']</t>
+          <t>['Italy', 'Czechoslovakia']</t>
         </is>
       </c>
       <c r="S54" t="n">
         <v>1</v>
       </c>
       <c r="T54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U54" t="n">
         <v>1766</v>
@@ -5083,7 +5083,7 @@
       <c r="I55" t="inlineStr"/>
       <c r="J55" t="inlineStr">
         <is>
-          <t>['Romania', 'Cameroon', 'Argentina']</t>
+          <t>['Cameroon', 'Argentina', 'Romania']</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -5167,7 +5167,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>['Romania', 'Cameroon', 'Argentina']</t>
+          <t>['Cameroon', 'Argentina', 'Romania']</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -5255,7 +5255,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>['Romania', 'Cameroon', 'Argentina']</t>
+          <t>['Cameroon', 'Argentina', 'Romania']</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -5343,7 +5343,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>['Romania', 'Cameroon', 'Argentina']</t>
+          <t>['Cameroon', 'Argentina', 'Romania']</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -5431,7 +5431,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>['Romania', 'Cameroon', 'Argentina']</t>
+          <t>['Cameroon', 'Romania', 'Argentina']</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -5519,7 +5519,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>['Romania', 'Cameroon', 'Argentina']</t>
+          <t>['Cameroon', 'Romania', 'Argentina']</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -5607,7 +5607,7 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>['Romania', 'Cameroon', 'Argentina']</t>
+          <t>['Cameroon', 'Argentina', 'Romania']</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
@@ -5681,7 +5681,7 @@
       <c r="I62" t="inlineStr"/>
       <c r="J62" t="inlineStr">
         <is>
-          <t>['Costa Rica', 'Brazil', 'Scotland']</t>
+          <t>['Costa Rica', 'Scotland', 'Brazil']</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
@@ -5765,7 +5765,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>['Scotland', 'Brazil', 'Sweden']</t>
+          <t>['Sweden', 'Scotland', 'Brazil']</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -5853,7 +5853,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>['Costa Rica', 'Brazil', 'Scotland']</t>
+          <t>['Costa Rica', 'Scotland', 'Brazil']</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -5941,7 +5941,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>['Costa Rica', 'Brazil', 'Scotland']</t>
+          <t>['Costa Rica', 'Scotland', 'Brazil']</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -6029,7 +6029,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>['Costa Rica', 'Brazil', 'Scotland']</t>
+          <t>['Costa Rica', 'Scotland', 'Brazil']</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -6103,7 +6103,7 @@
       <c r="I67" t="inlineStr"/>
       <c r="J67" t="inlineStr">
         <is>
-          <t>['Colombia', 'West Germany', 'Yugoslavia']</t>
+          <t>['Yugoslavia', 'Colombia', 'West Germany']</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -6187,7 +6187,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>['Colombia', 'West Germany', 'Yugoslavia']</t>
+          <t>['Yugoslavia', 'Colombia', 'West Germany']</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -6275,7 +6275,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>['Colombia', 'West Germany', 'Yugoslavia']</t>
+          <t>['Yugoslavia', 'Colombia', 'West Germany']</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -6363,7 +6363,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>['Colombia', 'West Germany', 'Yugoslavia']</t>
+          <t>['Yugoslavia', 'Colombia', 'West Germany']</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -6451,7 +6451,7 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>['Colombia', 'West Germany', 'Yugoslavia']</t>
+          <t>['Yugoslavia', 'Colombia', 'West Germany']</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
@@ -6539,7 +6539,7 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>['Colombia', 'West Germany', 'Yugoslavia']</t>
+          <t>['Yugoslavia', 'Colombia', 'West Germany']</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
@@ -6627,7 +6627,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>['Colombia', 'West Germany', 'Yugoslavia']</t>
+          <t>['Yugoslavia', 'Colombia', 'West Germany']</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -6715,7 +6715,7 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>['Colombia', 'West Germany', 'Yugoslavia']</t>
+          <t>['Yugoslavia', 'Colombia', 'West Germany']</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
@@ -6789,7 +6789,7 @@
       <c r="I75" t="inlineStr"/>
       <c r="J75" t="inlineStr">
         <is>
-          <t>['Belgium', 'Spain', 'Uruguay']</t>
+          <t>['Spain', 'Uruguay', 'Belgium']</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
@@ -6873,7 +6873,7 @@
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>['Belgium', 'Spain', 'Uruguay']</t>
+          <t>['Spain', 'Uruguay', 'Belgium']</t>
         </is>
       </c>
       <c r="K76" t="inlineStr">
@@ -6961,7 +6961,7 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>['Belgium', 'Spain', 'Uruguay']</t>
+          <t>['Spain', 'Uruguay', 'Belgium']</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
@@ -7049,7 +7049,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>['Belgium', 'Spain', 'Uruguay']</t>
+          <t>['Spain', 'Uruguay', 'Belgium']</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
@@ -7137,7 +7137,7 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>['Belgium', 'Spain', 'Uruguay']</t>
+          <t>['Spain', 'Uruguay', 'Belgium']</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
@@ -7211,7 +7211,7 @@
       <c r="I80" t="inlineStr"/>
       <c r="J80" t="inlineStr">
         <is>
-          <t>['England', 'Ireland', 'Netherlands']</t>
+          <t>['Ireland', 'Netherlands', 'England']</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -7295,7 +7295,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>['England', 'Egypt', 'Netherlands']</t>
+          <t>['Egypt', 'Netherlands', 'England']</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -7383,7 +7383,7 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>['England', 'Egypt', 'Netherlands']</t>
+          <t>['Egypt', 'Netherlands', 'England']</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
@@ -7471,7 +7471,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>['England', 'Ireland', 'Netherlands']</t>
+          <t>['Ireland', 'Netherlands', 'England']</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
@@ -7545,7 +7545,7 @@
       <c r="I84" t="inlineStr"/>
       <c r="J84" t="inlineStr">
         <is>
-          <t>['Switzerland', 'United States', 'Romania']</t>
+          <t>['United States', 'Romania', 'Switzerland']</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
@@ -7625,7 +7625,7 @@
       <c r="I85" t="inlineStr"/>
       <c r="J85" t="inlineStr">
         <is>
-          <t>['Switzerland', 'United States', 'Romania']</t>
+          <t>['United States', 'Romania', 'Switzerland']</t>
         </is>
       </c>
       <c r="K85" t="inlineStr">
@@ -7709,7 +7709,7 @@
       <c r="I86" t="inlineStr"/>
       <c r="J86" t="inlineStr">
         <is>
-          <t>['Switzerland', 'United States', 'Romania']</t>
+          <t>['United States', 'Romania', 'Switzerland']</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
@@ -7797,7 +7797,7 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>['Switzerland', 'United States', 'Romania']</t>
+          <t>['United States', 'Romania', 'Switzerland']</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
@@ -7885,7 +7885,7 @@
       </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>['Switzerland', 'United States', 'Romania']</t>
+          <t>['United States', 'Romania', 'Switzerland']</t>
         </is>
       </c>
       <c r="K88" t="inlineStr">
@@ -7973,7 +7973,7 @@
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>['Switzerland', 'United States', 'Romania']</t>
+          <t>['United States', 'Romania', 'Switzerland']</t>
         </is>
       </c>
       <c r="K89" t="inlineStr">
@@ -8047,7 +8047,7 @@
       <c r="I90" t="inlineStr"/>
       <c r="J90" t="inlineStr">
         <is>
-          <t>['Sweden', 'Brazil', 'Cameroon']</t>
+          <t>['Cameroon', 'Sweden', 'Brazil']</t>
         </is>
       </c>
       <c r="K90" t="inlineStr">
@@ -8131,7 +8131,7 @@
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>['Sweden', 'Brazil', 'Russia']</t>
+          <t>['Sweden', 'Russia', 'Brazil']</t>
         </is>
       </c>
       <c r="K91" t="inlineStr">
@@ -8219,7 +8219,7 @@
       </c>
       <c r="J92" t="inlineStr">
         <is>
-          <t>['Sweden', 'Brazil', 'Russia']</t>
+          <t>['Brazil', 'Russia', 'Sweden']</t>
         </is>
       </c>
       <c r="K92" t="inlineStr">
@@ -8307,7 +8307,7 @@
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>['Sweden', 'Brazil', 'Russia']</t>
+          <t>['Brazil', 'Russia', 'Sweden']</t>
         </is>
       </c>
       <c r="K93" t="inlineStr">
@@ -8395,7 +8395,7 @@
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>['Sweden', 'Brazil', 'Russia']</t>
+          <t>['Brazil', 'Russia', 'Sweden']</t>
         </is>
       </c>
       <c r="K94" t="inlineStr">
@@ -8483,7 +8483,7 @@
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>['Sweden', 'Brazil', 'Russia']</t>
+          <t>['Brazil', 'Russia', 'Sweden']</t>
         </is>
       </c>
       <c r="K95" t="inlineStr">
@@ -8571,7 +8571,7 @@
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>['Sweden', 'Brazil', 'Russia']</t>
+          <t>['Sweden', 'Russia', 'Brazil']</t>
         </is>
       </c>
       <c r="K96" t="inlineStr">
@@ -8659,7 +8659,7 @@
       </c>
       <c r="J97" t="inlineStr">
         <is>
-          <t>['Sweden', 'Brazil', 'Russia']</t>
+          <t>['Sweden', 'Russia', 'Brazil']</t>
         </is>
       </c>
       <c r="K97" t="inlineStr">
@@ -8747,7 +8747,7 @@
       </c>
       <c r="J98" t="inlineStr">
         <is>
-          <t>['Sweden', 'Brazil', 'Russia']</t>
+          <t>['Sweden', 'Russia', 'Brazil']</t>
         </is>
       </c>
       <c r="K98" t="inlineStr">
@@ -8835,7 +8835,7 @@
       </c>
       <c r="J99" t="inlineStr">
         <is>
-          <t>['Sweden', 'Brazil', 'Russia']</t>
+          <t>['Sweden', 'Russia', 'Brazil']</t>
         </is>
       </c>
       <c r="K99" t="inlineStr">
@@ -8909,7 +8909,7 @@
       <c r="I100" t="inlineStr"/>
       <c r="J100" t="inlineStr">
         <is>
-          <t>['South Korea', 'Spain', 'Germany']</t>
+          <t>['Germany', 'South Korea', 'Spain']</t>
         </is>
       </c>
       <c r="K100" t="inlineStr">
@@ -8993,7 +8993,7 @@
       </c>
       <c r="J101" t="inlineStr">
         <is>
-          <t>['South Korea', 'Spain', 'Germany']</t>
+          <t>['Germany', 'South Korea', 'Spain']</t>
         </is>
       </c>
       <c r="K101" t="inlineStr">
@@ -9081,7 +9081,7 @@
       </c>
       <c r="J102" t="inlineStr">
         <is>
-          <t>['South Korea', 'Spain', 'Germany']</t>
+          <t>['Germany', 'South Korea', 'Spain']</t>
         </is>
       </c>
       <c r="K102" t="inlineStr">
@@ -9169,7 +9169,7 @@
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>['South Korea', 'Spain', 'Germany']</t>
+          <t>['Germany', 'South Korea', 'Spain']</t>
         </is>
       </c>
       <c r="K103" t="inlineStr">
@@ -9257,7 +9257,7 @@
       </c>
       <c r="J104" t="inlineStr">
         <is>
-          <t>['South Korea', 'Spain', 'Germany']</t>
+          <t>['Germany', 'South Korea', 'Spain']</t>
         </is>
       </c>
       <c r="K104" t="inlineStr">
@@ -9345,7 +9345,7 @@
       </c>
       <c r="J105" t="inlineStr">
         <is>
-          <t>['South Korea', 'Spain', 'Germany']</t>
+          <t>['Germany', 'South Korea', 'Spain']</t>
         </is>
       </c>
       <c r="K105" t="inlineStr">
@@ -9433,7 +9433,7 @@
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>['South Korea', 'Spain', 'Germany']</t>
+          <t>['Germany', 'South Korea', 'Spain']</t>
         </is>
       </c>
       <c r="K106" t="inlineStr">
@@ -9521,7 +9521,7 @@
       </c>
       <c r="J107" t="inlineStr">
         <is>
-          <t>['South Korea', 'Spain', 'Germany']</t>
+          <t>['Germany', 'South Korea', 'Spain']</t>
         </is>
       </c>
       <c r="K107" t="inlineStr">
@@ -9609,7 +9609,7 @@
       </c>
       <c r="J108" t="inlineStr">
         <is>
-          <t>['South Korea', 'Spain', 'Germany']</t>
+          <t>['Germany', 'South Korea', 'Spain']</t>
         </is>
       </c>
       <c r="K108" t="inlineStr">
@@ -9697,7 +9697,7 @@
       </c>
       <c r="J109" t="inlineStr">
         <is>
-          <t>['South Korea', 'Spain', 'Germany']</t>
+          <t>['Germany', 'South Korea', 'Spain']</t>
         </is>
       </c>
       <c r="K109" t="inlineStr">
@@ -9771,7 +9771,7 @@
       <c r="I110" t="inlineStr"/>
       <c r="J110" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Nigeria', 'Argentina']</t>
+          <t>['Bulgaria', 'Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K110" t="inlineStr">
@@ -9851,7 +9851,7 @@
       <c r="I111" t="inlineStr"/>
       <c r="J111" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Nigeria', 'Argentina']</t>
+          <t>['Bulgaria', 'Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K111" t="inlineStr">
@@ -9935,7 +9935,7 @@
       <c r="I112" t="inlineStr"/>
       <c r="J112" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Nigeria', 'Argentina']</t>
+          <t>['Bulgaria', 'Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K112" t="inlineStr">
@@ -10023,7 +10023,7 @@
       </c>
       <c r="J113" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Nigeria', 'Argentina']</t>
+          <t>['Bulgaria', 'Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K113" t="inlineStr">
@@ -10111,7 +10111,7 @@
       </c>
       <c r="J114" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K114" t="inlineStr">
@@ -10361,7 +10361,7 @@
       <c r="I117" t="inlineStr"/>
       <c r="J117" t="inlineStr">
         <is>
-          <t>['Mexico', 'Italy', 'Norway']</t>
+          <t>['Norway', 'Mexico', 'Italy']</t>
         </is>
       </c>
       <c r="K117" t="inlineStr">
@@ -10441,7 +10441,7 @@
       <c r="I118" t="inlineStr"/>
       <c r="J118" t="inlineStr">
         <is>
-          <t>['Mexico', 'Ireland', 'Italy']</t>
+          <t>['Ireland', 'Mexico', 'Italy']</t>
         </is>
       </c>
       <c r="K118" t="inlineStr">
@@ -10617,7 +10617,7 @@
       </c>
       <c r="J120" t="inlineStr">
         <is>
-          <t>['Mexico', 'Ireland', 'Italy']</t>
+          <t>['Ireland', 'Mexico', 'Italy']</t>
         </is>
       </c>
       <c r="K120" t="inlineStr">
@@ -10691,7 +10691,7 @@
       <c r="I121" t="inlineStr"/>
       <c r="J121" t="inlineStr">
         <is>
-          <t>['Belgium', 'Saudi Arabia', 'Netherlands']</t>
+          <t>['Saudi Arabia', 'Netherlands', 'Belgium']</t>
         </is>
       </c>
       <c r="K121" t="inlineStr">
@@ -10771,7 +10771,7 @@
       <c r="I122" t="inlineStr"/>
       <c r="J122" t="inlineStr">
         <is>
-          <t>['Belgium', 'Saudi Arabia', 'Netherlands']</t>
+          <t>['Saudi Arabia', 'Netherlands', 'Belgium']</t>
         </is>
       </c>
       <c r="K122" t="inlineStr">
@@ -11197,7 +11197,7 @@
       <c r="I127" t="inlineStr"/>
       <c r="J127" t="inlineStr">
         <is>
-          <t>['Brazil', 'Norway']</t>
+          <t>['Norway', 'Brazil']</t>
         </is>
       </c>
       <c r="K127" t="inlineStr">
@@ -11277,7 +11277,7 @@
       <c r="I128" t="inlineStr"/>
       <c r="J128" t="inlineStr">
         <is>
-          <t>['Brazil', 'Norway']</t>
+          <t>['Norway', 'Brazil']</t>
         </is>
       </c>
       <c r="K128" t="inlineStr">
@@ -11365,7 +11365,7 @@
       </c>
       <c r="J129" t="inlineStr">
         <is>
-          <t>['Brazil', 'Morocco']</t>
+          <t>['Morocco', 'Brazil']</t>
         </is>
       </c>
       <c r="K129" t="inlineStr">
@@ -11453,7 +11453,7 @@
       </c>
       <c r="J130" t="inlineStr">
         <is>
-          <t>['Brazil', 'Morocco']</t>
+          <t>['Morocco', 'Brazil']</t>
         </is>
       </c>
       <c r="K130" t="inlineStr">
@@ -11541,7 +11541,7 @@
       </c>
       <c r="J131" t="inlineStr">
         <is>
-          <t>['Brazil', 'Morocco']</t>
+          <t>['Morocco', 'Brazil']</t>
         </is>
       </c>
       <c r="K131" t="inlineStr">
@@ -11629,7 +11629,7 @@
       </c>
       <c r="J132" t="inlineStr">
         <is>
-          <t>['Brazil', 'Morocco']</t>
+          <t>['Morocco', 'Brazil']</t>
         </is>
       </c>
       <c r="K132" t="inlineStr">
@@ -11717,7 +11717,7 @@
       </c>
       <c r="J133" t="inlineStr">
         <is>
-          <t>['Brazil', 'Morocco']</t>
+          <t>['Morocco', 'Brazil']</t>
         </is>
       </c>
       <c r="K133" t="inlineStr">
@@ -11805,7 +11805,7 @@
       </c>
       <c r="J134" t="inlineStr">
         <is>
-          <t>['Brazil', 'Norway']</t>
+          <t>['Norway', 'Brazil']</t>
         </is>
       </c>
       <c r="K134" t="inlineStr">
@@ -11879,7 +11879,7 @@
       <c r="I135" t="inlineStr"/>
       <c r="J135" t="inlineStr">
         <is>
-          <t>['Italy', 'Chile']</t>
+          <t>['Chile', 'Italy']</t>
         </is>
       </c>
       <c r="K135" t="inlineStr">
@@ -11963,7 +11963,7 @@
       </c>
       <c r="J136" t="inlineStr">
         <is>
-          <t>['Italy', 'Chile']</t>
+          <t>['Chile', 'Italy']</t>
         </is>
       </c>
       <c r="K136" t="inlineStr">
@@ -12055,7 +12055,7 @@
       </c>
       <c r="J137" t="inlineStr">
         <is>
-          <t>['Italy', 'Chile']</t>
+          <t>['Chile', 'Italy']</t>
         </is>
       </c>
       <c r="K137" t="inlineStr">
@@ -12143,7 +12143,7 @@
       </c>
       <c r="J138" t="inlineStr">
         <is>
-          <t>['Italy', 'Chile']</t>
+          <t>['Chile', 'Italy']</t>
         </is>
       </c>
       <c r="K138" t="inlineStr">
@@ -12231,7 +12231,7 @@
       </c>
       <c r="J139" t="inlineStr">
         <is>
-          <t>['Italy', 'Chile']</t>
+          <t>['Chile', 'Italy']</t>
         </is>
       </c>
       <c r="K139" t="inlineStr">
@@ -12319,7 +12319,7 @@
       </c>
       <c r="J140" t="inlineStr">
         <is>
-          <t>['Italy', 'Chile']</t>
+          <t>['Chile', 'Italy']</t>
         </is>
       </c>
       <c r="K140" t="inlineStr">
@@ -14289,7 +14289,7 @@
       </c>
       <c r="J163" t="inlineStr">
         <is>
-          <t>['Belgium', 'Netherlands']</t>
+          <t>['Netherlands', 'Belgium']</t>
         </is>
       </c>
       <c r="K163" t="inlineStr">
@@ -14377,7 +14377,7 @@
       </c>
       <c r="J164" t="inlineStr">
         <is>
-          <t>['Belgium', 'Netherlands']</t>
+          <t>['Netherlands', 'Belgium']</t>
         </is>
       </c>
       <c r="K164" t="inlineStr">
@@ -15217,7 +15217,7 @@
       <c r="I174" t="inlineStr"/>
       <c r="J174" t="inlineStr">
         <is>
-          <t>['England', 'Romania']</t>
+          <t>['Romania', 'England']</t>
         </is>
       </c>
       <c r="K174" t="inlineStr">
@@ -15297,7 +15297,7 @@
       <c r="I175" t="inlineStr"/>
       <c r="J175" t="inlineStr">
         <is>
-          <t>['England', 'Romania']</t>
+          <t>['Romania', 'England']</t>
         </is>
       </c>
       <c r="K175" t="inlineStr">
@@ -15385,7 +15385,7 @@
       </c>
       <c r="J176" t="inlineStr">
         <is>
-          <t>['England', 'Romania']</t>
+          <t>['Romania', 'England']</t>
         </is>
       </c>
       <c r="K176" t="inlineStr">
@@ -15473,7 +15473,7 @@
       </c>
       <c r="J177" t="inlineStr">
         <is>
-          <t>['England', 'Romania']</t>
+          <t>['Romania', 'England']</t>
         </is>
       </c>
       <c r="K177" t="inlineStr">
@@ -15561,7 +15561,7 @@
       </c>
       <c r="J178" t="inlineStr">
         <is>
-          <t>['England', 'Romania']</t>
+          <t>['Romania', 'England']</t>
         </is>
       </c>
       <c r="K178" t="inlineStr">
@@ -15649,7 +15649,7 @@
       </c>
       <c r="J179" t="inlineStr">
         <is>
-          <t>['England', 'Romania']</t>
+          <t>['Romania', 'England']</t>
         </is>
       </c>
       <c r="K179" t="inlineStr">
@@ -16397,7 +16397,7 @@
       </c>
       <c r="J188" t="inlineStr">
         <is>
-          <t>['Denmark', 'Senegal']</t>
+          <t>['Senegal', 'Denmark']</t>
         </is>
       </c>
       <c r="K188" t="inlineStr">
@@ -16573,7 +16573,7 @@
       </c>
       <c r="J190" t="inlineStr">
         <is>
-          <t>['Denmark', 'Senegal']</t>
+          <t>['Senegal', 'Denmark']</t>
         </is>
       </c>
       <c r="K190" t="inlineStr">
@@ -16661,7 +16661,7 @@
       </c>
       <c r="J191" t="inlineStr">
         <is>
-          <t>['Denmark', 'Senegal']</t>
+          <t>['Senegal', 'Denmark']</t>
         </is>
       </c>
       <c r="K191" t="inlineStr">
@@ -16749,7 +16749,7 @@
       </c>
       <c r="J192" t="inlineStr">
         <is>
-          <t>['Denmark', 'Senegal']</t>
+          <t>['Senegal', 'Denmark']</t>
         </is>
       </c>
       <c r="K192" t="inlineStr">
@@ -16837,7 +16837,7 @@
       </c>
       <c r="J193" t="inlineStr">
         <is>
-          <t>['Denmark', 'Senegal']</t>
+          <t>['Senegal', 'Denmark']</t>
         </is>
       </c>
       <c r="K193" t="inlineStr">
@@ -17087,7 +17087,7 @@
       <c r="I196" t="inlineStr"/>
       <c r="J196" t="inlineStr">
         <is>
-          <t>['South Africa', 'Spain']</t>
+          <t>['Spain', 'South Africa']</t>
         </is>
       </c>
       <c r="K196" t="inlineStr">
@@ -17171,7 +17171,7 @@
       </c>
       <c r="J197" t="inlineStr">
         <is>
-          <t>['South Africa', 'Spain']</t>
+          <t>['Spain', 'South Africa']</t>
         </is>
       </c>
       <c r="K197" t="inlineStr">
@@ -17259,7 +17259,7 @@
       </c>
       <c r="J198" t="inlineStr">
         <is>
-          <t>['South Africa', 'Spain']</t>
+          <t>['Spain', 'South Africa']</t>
         </is>
       </c>
       <c r="K198" t="inlineStr">
@@ -17347,7 +17347,7 @@
       </c>
       <c r="J199" t="inlineStr">
         <is>
-          <t>['South Africa', 'Spain']</t>
+          <t>['Spain', 'South Africa']</t>
         </is>
       </c>
       <c r="K199" t="inlineStr">
@@ -17435,7 +17435,7 @@
       </c>
       <c r="J200" t="inlineStr">
         <is>
-          <t>['South Africa', 'Spain']</t>
+          <t>['Spain', 'South Africa']</t>
         </is>
       </c>
       <c r="K200" t="inlineStr">
@@ -17523,7 +17523,7 @@
       </c>
       <c r="J201" t="inlineStr">
         <is>
-          <t>['South Africa', 'Spain']</t>
+          <t>['Spain', 'South Africa']</t>
         </is>
       </c>
       <c r="K201" t="inlineStr">
@@ -17611,7 +17611,7 @@
       </c>
       <c r="J202" t="inlineStr">
         <is>
-          <t>['South Africa', 'Spain']</t>
+          <t>['Spain', 'South Africa']</t>
         </is>
       </c>
       <c r="K202" t="inlineStr">
@@ -17699,7 +17699,7 @@
       </c>
       <c r="J203" t="inlineStr">
         <is>
-          <t>['South Africa', 'Spain']</t>
+          <t>['Spain', 'South Africa']</t>
         </is>
       </c>
       <c r="K203" t="inlineStr">
@@ -17787,7 +17787,7 @@
       </c>
       <c r="J204" t="inlineStr">
         <is>
-          <t>['South Africa', 'Spain']</t>
+          <t>['Spain', 'South Africa']</t>
         </is>
       </c>
       <c r="K204" t="inlineStr">
@@ -18983,7 +18983,7 @@
       <c r="I218" t="inlineStr"/>
       <c r="J218" t="inlineStr">
         <is>
-          <t>['South Korea', 'United States']</t>
+          <t>['United States', 'South Korea']</t>
         </is>
       </c>
       <c r="K218" t="inlineStr">
@@ -19063,7 +19063,7 @@
       <c r="I219" t="inlineStr"/>
       <c r="J219" t="inlineStr">
         <is>
-          <t>['South Korea', 'United States']</t>
+          <t>['United States', 'South Korea']</t>
         </is>
       </c>
       <c r="K219" t="inlineStr">
@@ -19151,7 +19151,7 @@
       </c>
       <c r="J220" t="inlineStr">
         <is>
-          <t>['South Korea', 'United States']</t>
+          <t>['United States', 'South Korea']</t>
         </is>
       </c>
       <c r="K220" t="inlineStr">
@@ -19239,7 +19239,7 @@
       </c>
       <c r="J221" t="inlineStr">
         <is>
-          <t>['South Korea', 'United States']</t>
+          <t>['United States', 'South Korea']</t>
         </is>
       </c>
       <c r="K221" t="inlineStr">
@@ -19327,7 +19327,7 @@
       </c>
       <c r="J222" t="inlineStr">
         <is>
-          <t>['South Korea', 'United States']</t>
+          <t>['United States', 'South Korea']</t>
         </is>
       </c>
       <c r="K222" t="inlineStr">
@@ -19415,7 +19415,7 @@
       </c>
       <c r="J223" t="inlineStr">
         <is>
-          <t>['South Korea', 'United States']</t>
+          <t>['United States', 'South Korea']</t>
         </is>
       </c>
       <c r="K223" t="inlineStr">
@@ -19503,7 +19503,7 @@
       </c>
       <c r="J224" t="inlineStr">
         <is>
-          <t>['South Korea', 'United States']</t>
+          <t>['United States', 'South Korea']</t>
         </is>
       </c>
       <c r="K224" t="inlineStr">
@@ -19837,7 +19837,7 @@
       </c>
       <c r="J228" t="inlineStr">
         <is>
-          <t>['Ireland', 'Germany']</t>
+          <t>['Germany', 'Ireland']</t>
         </is>
       </c>
       <c r="K228" t="inlineStr">
@@ -19925,7 +19925,7 @@
       </c>
       <c r="J229" t="inlineStr">
         <is>
-          <t>['Ireland', 'Germany']</t>
+          <t>['Germany', 'Ireland']</t>
         </is>
       </c>
       <c r="K229" t="inlineStr">
@@ -20013,7 +20013,7 @@
       </c>
       <c r="J230" t="inlineStr">
         <is>
-          <t>['Ireland', 'Germany']</t>
+          <t>['Germany', 'Ireland']</t>
         </is>
       </c>
       <c r="K230" t="inlineStr">
@@ -20101,7 +20101,7 @@
       </c>
       <c r="J231" t="inlineStr">
         <is>
-          <t>['Ireland', 'Germany']</t>
+          <t>['Germany', 'Ireland']</t>
         </is>
       </c>
       <c r="K231" t="inlineStr">
@@ -20189,7 +20189,7 @@
       </c>
       <c r="J232" t="inlineStr">
         <is>
-          <t>['Ireland', 'Germany']</t>
+          <t>['Germany', 'Ireland']</t>
         </is>
       </c>
       <c r="K232" t="inlineStr">
@@ -20263,7 +20263,7 @@
       <c r="I233" t="inlineStr"/>
       <c r="J233" t="inlineStr">
         <is>
-          <t>['Sweden', 'England']</t>
+          <t>['England', 'Sweden']</t>
         </is>
       </c>
       <c r="K233" t="inlineStr">
@@ -20343,7 +20343,7 @@
       <c r="I234" t="inlineStr"/>
       <c r="J234" t="inlineStr">
         <is>
-          <t>['Sweden', 'England']</t>
+          <t>['England', 'Sweden']</t>
         </is>
       </c>
       <c r="K234" t="inlineStr">
@@ -20431,7 +20431,7 @@
       </c>
       <c r="J235" t="inlineStr">
         <is>
-          <t>['Sweden', 'England']</t>
+          <t>['England', 'Sweden']</t>
         </is>
       </c>
       <c r="K235" t="inlineStr">
@@ -20519,7 +20519,7 @@
       </c>
       <c r="J236" t="inlineStr">
         <is>
-          <t>['Sweden', 'England']</t>
+          <t>['England', 'Sweden']</t>
         </is>
       </c>
       <c r="K236" t="inlineStr">
@@ -20593,7 +20593,7 @@
       <c r="I237" t="inlineStr"/>
       <c r="J237" t="inlineStr">
         <is>
-          <t>['Mexico', 'Croatia']</t>
+          <t>['Croatia', 'Mexico']</t>
         </is>
       </c>
       <c r="K237" t="inlineStr">
@@ -20673,7 +20673,7 @@
       <c r="I238" t="inlineStr"/>
       <c r="J238" t="inlineStr">
         <is>
-          <t>['Mexico', 'Croatia']</t>
+          <t>['Croatia', 'Mexico']</t>
         </is>
       </c>
       <c r="K238" t="inlineStr">
@@ -20761,7 +20761,7 @@
       </c>
       <c r="J239" t="inlineStr">
         <is>
-          <t>['Mexico', 'Croatia']</t>
+          <t>['Croatia', 'Mexico']</t>
         </is>
       </c>
       <c r="K239" t="inlineStr">
@@ -21179,7 +21179,7 @@
       </c>
       <c r="J244" t="inlineStr">
         <is>
-          <t>['Belgium', 'Japan']</t>
+          <t>['Japan', 'Belgium']</t>
         </is>
       </c>
       <c r="K244" t="inlineStr">
@@ -21267,7 +21267,7 @@
       </c>
       <c r="J245" t="inlineStr">
         <is>
-          <t>['Belgium', 'Japan']</t>
+          <t>['Japan', 'Belgium']</t>
         </is>
       </c>
       <c r="K245" t="inlineStr">
@@ -21531,7 +21531,7 @@
       </c>
       <c r="J248" t="inlineStr">
         <is>
-          <t>['Belgium', 'Japan']</t>
+          <t>['Japan', 'Belgium']</t>
         </is>
       </c>
       <c r="K248" t="inlineStr">
@@ -21619,7 +21619,7 @@
       </c>
       <c r="J249" t="inlineStr">
         <is>
-          <t>['Belgium', 'Japan']</t>
+          <t>['Japan', 'Belgium']</t>
         </is>
       </c>
       <c r="K249" t="inlineStr">
@@ -21707,7 +21707,7 @@
       </c>
       <c r="J250" t="inlineStr">
         <is>
-          <t>['Belgium', 'Japan']</t>
+          <t>['Japan', 'Belgium']</t>
         </is>
       </c>
       <c r="K250" t="inlineStr">
@@ -22463,7 +22463,7 @@
       <c r="I259" t="inlineStr"/>
       <c r="J259" t="inlineStr">
         <is>
-          <t>['England', 'Sweden']</t>
+          <t>['Sweden', 'England']</t>
         </is>
       </c>
       <c r="K259" t="inlineStr">
@@ -22543,7 +22543,7 @@
       <c r="I260" t="inlineStr"/>
       <c r="J260" t="inlineStr">
         <is>
-          <t>['England', 'Sweden']</t>
+          <t>['Sweden', 'England']</t>
         </is>
       </c>
       <c r="K260" t="inlineStr">
@@ -22631,7 +22631,7 @@
       </c>
       <c r="J261" t="inlineStr">
         <is>
-          <t>['England', 'Sweden']</t>
+          <t>['Sweden', 'England']</t>
         </is>
       </c>
       <c r="K261" t="inlineStr">
@@ -22719,7 +22719,7 @@
       </c>
       <c r="J262" t="inlineStr">
         <is>
-          <t>['England', 'Sweden']</t>
+          <t>['Sweden', 'England']</t>
         </is>
       </c>
       <c r="K262" t="inlineStr">
@@ -22807,7 +22807,7 @@
       </c>
       <c r="J263" t="inlineStr">
         <is>
-          <t>['England', 'Sweden']</t>
+          <t>['Sweden', 'England']</t>
         </is>
       </c>
       <c r="K263" t="inlineStr">
@@ -22895,7 +22895,7 @@
       </c>
       <c r="J264" t="inlineStr">
         <is>
-          <t>['England', 'Sweden']</t>
+          <t>['Sweden', 'England']</t>
         </is>
       </c>
       <c r="K264" t="inlineStr">
@@ -22983,7 +22983,7 @@
       </c>
       <c r="J265" t="inlineStr">
         <is>
-          <t>['England', 'Sweden']</t>
+          <t>['Sweden', 'England']</t>
         </is>
       </c>
       <c r="K265" t="inlineStr">
@@ -23071,7 +23071,7 @@
       </c>
       <c r="J266" t="inlineStr">
         <is>
-          <t>['England', 'Sweden']</t>
+          <t>['Sweden', 'England']</t>
         </is>
       </c>
       <c r="K266" t="inlineStr">
@@ -23145,7 +23145,7 @@
       <c r="I267" t="inlineStr"/>
       <c r="J267" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Argentina']</t>
+          <t>['Argentina', 'Netherlands']</t>
         </is>
       </c>
       <c r="K267" t="inlineStr">
@@ -23225,7 +23225,7 @@
       <c r="I268" t="inlineStr"/>
       <c r="J268" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Argentina']</t>
+          <t>['Argentina', 'Netherlands']</t>
         </is>
       </c>
       <c r="K268" t="inlineStr">
@@ -23313,7 +23313,7 @@
       </c>
       <c r="J269" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Argentina']</t>
+          <t>['Argentina', 'Netherlands']</t>
         </is>
       </c>
       <c r="K269" t="inlineStr">
@@ -23401,7 +23401,7 @@
       </c>
       <c r="J270" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Argentina']</t>
+          <t>['Argentina', 'Netherlands']</t>
         </is>
       </c>
       <c r="K270" t="inlineStr">
@@ -23489,7 +23489,7 @@
       </c>
       <c r="J271" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Argentina']</t>
+          <t>['Argentina', 'Netherlands']</t>
         </is>
       </c>
       <c r="K271" t="inlineStr">
@@ -23577,7 +23577,7 @@
       </c>
       <c r="J272" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Argentina']</t>
+          <t>['Argentina', 'Netherlands']</t>
         </is>
       </c>
       <c r="K272" t="inlineStr">
@@ -23665,7 +23665,7 @@
       </c>
       <c r="J273" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Argentina']</t>
+          <t>['Argentina', 'Netherlands']</t>
         </is>
       </c>
       <c r="K273" t="inlineStr">
@@ -23739,7 +23739,7 @@
       <c r="I274" t="inlineStr"/>
       <c r="J274" t="inlineStr">
         <is>
-          <t>['Mexico', 'Portugal']</t>
+          <t>['Portugal', 'Mexico']</t>
         </is>
       </c>
       <c r="K274" t="inlineStr">
@@ -23823,7 +23823,7 @@
       </c>
       <c r="J275" t="inlineStr">
         <is>
-          <t>['Mexico', 'Portugal']</t>
+          <t>['Portugal', 'Mexico']</t>
         </is>
       </c>
       <c r="K275" t="inlineStr">
@@ -23911,7 +23911,7 @@
       </c>
       <c r="J276" t="inlineStr">
         <is>
-          <t>['Mexico', 'Portugal']</t>
+          <t>['Portugal', 'Mexico']</t>
         </is>
       </c>
       <c r="K276" t="inlineStr">
@@ -24003,7 +24003,7 @@
       </c>
       <c r="J277" t="inlineStr">
         <is>
-          <t>['Mexico', 'Portugal']</t>
+          <t>['Portugal', 'Mexico']</t>
         </is>
       </c>
       <c r="K277" t="inlineStr">
@@ -24091,7 +24091,7 @@
       </c>
       <c r="J278" t="inlineStr">
         <is>
-          <t>['Mexico', 'Portugal']</t>
+          <t>['Portugal', 'Mexico']</t>
         </is>
       </c>
       <c r="K278" t="inlineStr">
@@ -24179,7 +24179,7 @@
       </c>
       <c r="J279" t="inlineStr">
         <is>
-          <t>['Mexico', 'Portugal']</t>
+          <t>['Portugal', 'Mexico']</t>
         </is>
       </c>
       <c r="K279" t="inlineStr">
@@ -24253,7 +24253,7 @@
       <c r="I280" t="inlineStr"/>
       <c r="J280" t="inlineStr">
         <is>
-          <t>['Italy', 'Ghana']</t>
+          <t>['Ghana', 'Italy']</t>
         </is>
       </c>
       <c r="K280" t="inlineStr">
@@ -24333,7 +24333,7 @@
       <c r="I281" t="inlineStr"/>
       <c r="J281" t="inlineStr">
         <is>
-          <t>['Italy', 'Ghana']</t>
+          <t>['Ghana', 'Italy']</t>
         </is>
       </c>
       <c r="K281" t="inlineStr">
@@ -24421,7 +24421,7 @@
       </c>
       <c r="J282" t="inlineStr">
         <is>
-          <t>['Italy', 'Ghana']</t>
+          <t>['Ghana', 'Italy']</t>
         </is>
       </c>
       <c r="K282" t="inlineStr">
@@ -24509,7 +24509,7 @@
       </c>
       <c r="J283" t="inlineStr">
         <is>
-          <t>['Italy', 'Ghana']</t>
+          <t>['Ghana', 'Italy']</t>
         </is>
       </c>
       <c r="K283" t="inlineStr">
@@ -24597,7 +24597,7 @@
       </c>
       <c r="J284" t="inlineStr">
         <is>
-          <t>['Italy', 'Ghana']</t>
+          <t>['Ghana', 'Italy']</t>
         </is>
       </c>
       <c r="K284" t="inlineStr">
@@ -24685,7 +24685,7 @@
       </c>
       <c r="J285" t="inlineStr">
         <is>
-          <t>['Italy', 'Ghana']</t>
+          <t>['Ghana', 'Italy']</t>
         </is>
       </c>
       <c r="K285" t="inlineStr">
@@ -24773,7 +24773,7 @@
       </c>
       <c r="J286" t="inlineStr">
         <is>
-          <t>['Italy', 'Ghana']</t>
+          <t>['Ghana', 'Italy']</t>
         </is>
       </c>
       <c r="K286" t="inlineStr">
@@ -24847,7 +24847,7 @@
       <c r="I287" t="inlineStr"/>
       <c r="J287" t="inlineStr">
         <is>
-          <t>['Brazil', 'Australia']</t>
+          <t>['Australia', 'Brazil']</t>
         </is>
       </c>
       <c r="K287" t="inlineStr">
@@ -25107,7 +25107,7 @@
       </c>
       <c r="J290" t="inlineStr">
         <is>
-          <t>['Brazil', 'Australia']</t>
+          <t>['Australia', 'Brazil']</t>
         </is>
       </c>
       <c r="K290" t="inlineStr">
@@ -25195,7 +25195,7 @@
       </c>
       <c r="J291" t="inlineStr">
         <is>
-          <t>['Brazil', 'Australia']</t>
+          <t>['Australia', 'Brazil']</t>
         </is>
       </c>
       <c r="K291" t="inlineStr">
@@ -25287,7 +25287,7 @@
       </c>
       <c r="J292" t="inlineStr">
         <is>
-          <t>['Brazil', 'Australia']</t>
+          <t>['Australia', 'Brazil']</t>
         </is>
       </c>
       <c r="K292" t="inlineStr">
@@ -25555,7 +25555,7 @@
       </c>
       <c r="J295" t="inlineStr">
         <is>
-          <t>['Brazil', 'Australia']</t>
+          <t>['Australia', 'Brazil']</t>
         </is>
       </c>
       <c r="K295" t="inlineStr">
@@ -25647,7 +25647,7 @@
       </c>
       <c r="J296" t="inlineStr">
         <is>
-          <t>['Brazil', 'Australia']</t>
+          <t>['Australia', 'Brazil']</t>
         </is>
       </c>
       <c r="K296" t="inlineStr">
@@ -26073,7 +26073,7 @@
       </c>
       <c r="J301" t="inlineStr">
         <is>
-          <t>['Switzerland', 'France']</t>
+          <t>['France', 'Switzerland']</t>
         </is>
       </c>
       <c r="K301" t="inlineStr">
@@ -26161,7 +26161,7 @@
       </c>
       <c r="J302" t="inlineStr">
         <is>
-          <t>['Switzerland', 'France']</t>
+          <t>['France', 'Switzerland']</t>
         </is>
       </c>
       <c r="K302" t="inlineStr">
@@ -26249,7 +26249,7 @@
       </c>
       <c r="J303" t="inlineStr">
         <is>
-          <t>['Switzerland', 'France']</t>
+          <t>['France', 'Switzerland']</t>
         </is>
       </c>
       <c r="K303" t="inlineStr">
@@ -26737,7 +26737,7 @@
       <c r="I309" t="inlineStr"/>
       <c r="J309" t="inlineStr">
         <is>
-          <t>['Mexico', 'Uruguay']</t>
+          <t>['Uruguay', 'Mexico']</t>
         </is>
       </c>
       <c r="K309" t="inlineStr">
@@ -26817,7 +26817,7 @@
       <c r="I310" t="inlineStr"/>
       <c r="J310" t="inlineStr">
         <is>
-          <t>['Mexico', 'Uruguay']</t>
+          <t>['Uruguay', 'Mexico']</t>
         </is>
       </c>
       <c r="K310" t="inlineStr">
@@ -26905,7 +26905,7 @@
       </c>
       <c r="J311" t="inlineStr">
         <is>
-          <t>['Mexico', 'Uruguay']</t>
+          <t>['Uruguay', 'Mexico']</t>
         </is>
       </c>
       <c r="K311" t="inlineStr">
@@ -26993,7 +26993,7 @@
       </c>
       <c r="J312" t="inlineStr">
         <is>
-          <t>['Mexico', 'Uruguay']</t>
+          <t>['Uruguay', 'Mexico']</t>
         </is>
       </c>
       <c r="K312" t="inlineStr">
@@ -27081,7 +27081,7 @@
       </c>
       <c r="J313" t="inlineStr">
         <is>
-          <t>['Mexico', 'Uruguay']</t>
+          <t>['Uruguay', 'Mexico']</t>
         </is>
       </c>
       <c r="K313" t="inlineStr">
@@ -27169,7 +27169,7 @@
       </c>
       <c r="J314" t="inlineStr">
         <is>
-          <t>['Mexico', 'Uruguay']</t>
+          <t>['Uruguay', 'Mexico']</t>
         </is>
       </c>
       <c r="K314" t="inlineStr">
@@ -27411,7 +27411,7 @@
       </c>
       <c r="J317" t="inlineStr">
         <is>
-          <t>['Greece', 'Argentina']</t>
+          <t>['Argentina', 'Greece']</t>
         </is>
       </c>
       <c r="K317" t="inlineStr">
@@ -28181,7 +28181,7 @@
       </c>
       <c r="J326" t="inlineStr">
         <is>
-          <t>['England', 'Slovenia']</t>
+          <t>['Slovenia', 'England']</t>
         </is>
       </c>
       <c r="K326" t="inlineStr">
@@ -28269,7 +28269,7 @@
       </c>
       <c r="J327" t="inlineStr">
         <is>
-          <t>['England', 'United States']</t>
+          <t>['United States', 'England']</t>
         </is>
       </c>
       <c r="K327" t="inlineStr">
@@ -28343,7 +28343,7 @@
       <c r="I328" t="inlineStr"/>
       <c r="J328" t="inlineStr">
         <is>
-          <t>['Serbia', 'Ghana']</t>
+          <t>['Ghana', 'Serbia']</t>
         </is>
       </c>
       <c r="K328" t="inlineStr">
@@ -28423,7 +28423,7 @@
       <c r="I329" t="inlineStr"/>
       <c r="J329" t="inlineStr">
         <is>
-          <t>['Serbia', 'Ghana']</t>
+          <t>['Ghana', 'Serbia']</t>
         </is>
       </c>
       <c r="K329" t="inlineStr">
@@ -28511,7 +28511,7 @@
       </c>
       <c r="J330" t="inlineStr">
         <is>
-          <t>['Ghana', 'Germany']</t>
+          <t>['Germany', 'Ghana']</t>
         </is>
       </c>
       <c r="K330" t="inlineStr">
@@ -28599,7 +28599,7 @@
       </c>
       <c r="J331" t="inlineStr">
         <is>
-          <t>['Ghana', 'Germany']</t>
+          <t>['Germany', 'Ghana']</t>
         </is>
       </c>
       <c r="K331" t="inlineStr">
@@ -28687,7 +28687,7 @@
       </c>
       <c r="J332" t="inlineStr">
         <is>
-          <t>['Ghana', 'Germany']</t>
+          <t>['Germany', 'Ghana']</t>
         </is>
       </c>
       <c r="K332" t="inlineStr">
@@ -28775,7 +28775,7 @@
       </c>
       <c r="J333" t="inlineStr">
         <is>
-          <t>['Ghana', 'Germany']</t>
+          <t>['Germany', 'Ghana']</t>
         </is>
       </c>
       <c r="K333" t="inlineStr">
@@ -29535,7 +29535,7 @@
       <c r="I342" t="inlineStr"/>
       <c r="J342" t="inlineStr">
         <is>
-          <t>['Italy', 'Paraguay']</t>
+          <t>['Paraguay', 'Italy']</t>
         </is>
       </c>
       <c r="K342" t="inlineStr">
@@ -29615,7 +29615,7 @@
       <c r="I343" t="inlineStr"/>
       <c r="J343" t="inlineStr">
         <is>
-          <t>['Italy', 'Paraguay']</t>
+          <t>['Paraguay', 'Italy']</t>
         </is>
       </c>
       <c r="K343" t="inlineStr">
@@ -29703,7 +29703,7 @@
       </c>
       <c r="J344" t="inlineStr">
         <is>
-          <t>['Paraguay', 'Slovakia']</t>
+          <t>['Slovakia', 'Paraguay']</t>
         </is>
       </c>
       <c r="K344" t="inlineStr">
@@ -29791,7 +29791,7 @@
       </c>
       <c r="J345" t="inlineStr">
         <is>
-          <t>['Paraguay', 'Slovakia']</t>
+          <t>['Slovakia', 'Paraguay']</t>
         </is>
       </c>
       <c r="K345" t="inlineStr">
@@ -29879,7 +29879,7 @@
       </c>
       <c r="J346" t="inlineStr">
         <is>
-          <t>['Paraguay', 'Slovakia']</t>
+          <t>['Slovakia', 'Paraguay']</t>
         </is>
       </c>
       <c r="K346" t="inlineStr">
@@ -29967,7 +29967,7 @@
       </c>
       <c r="J347" t="inlineStr">
         <is>
-          <t>['Paraguay', 'Slovakia']</t>
+          <t>['Slovakia', 'Paraguay']</t>
         </is>
       </c>
       <c r="K347" t="inlineStr">
@@ -30055,7 +30055,7 @@
       </c>
       <c r="J348" t="inlineStr">
         <is>
-          <t>['Paraguay', 'Slovakia']</t>
+          <t>['Slovakia', 'Paraguay']</t>
         </is>
       </c>
       <c r="K348" t="inlineStr">
@@ -30129,7 +30129,7 @@
       <c r="I349" t="inlineStr"/>
       <c r="J349" t="inlineStr">
         <is>
-          <t>['Brazil', 'Portugal']</t>
+          <t>['Portugal', 'Brazil']</t>
         </is>
       </c>
       <c r="K349" t="inlineStr">
@@ -30209,7 +30209,7 @@
       <c r="I350" t="inlineStr"/>
       <c r="J350" t="inlineStr">
         <is>
-          <t>['Brazil', 'Portugal']</t>
+          <t>['Portugal', 'Brazil']</t>
         </is>
       </c>
       <c r="K350" t="inlineStr">
@@ -30293,7 +30293,7 @@
       <c r="I351" t="inlineStr"/>
       <c r="J351" t="inlineStr">
         <is>
-          <t>['Brazil', 'Portugal']</t>
+          <t>['Portugal', 'Brazil']</t>
         </is>
       </c>
       <c r="K351" t="inlineStr">
@@ -30381,7 +30381,7 @@
       </c>
       <c r="J352" t="inlineStr">
         <is>
-          <t>['Brazil', 'Portugal']</t>
+          <t>['Portugal', 'Brazil']</t>
         </is>
       </c>
       <c r="K352" t="inlineStr">
@@ -30469,7 +30469,7 @@
       </c>
       <c r="J353" t="inlineStr">
         <is>
-          <t>['Brazil', 'Portugal']</t>
+          <t>['Portugal', 'Brazil']</t>
         </is>
       </c>
       <c r="K353" t="inlineStr">
@@ -30557,7 +30557,7 @@
       </c>
       <c r="J354" t="inlineStr">
         <is>
-          <t>['Brazil', 'Portugal']</t>
+          <t>['Portugal', 'Brazil']</t>
         </is>
       </c>
       <c r="K354" t="inlineStr">
@@ -30631,7 +30631,7 @@
       <c r="I355" t="inlineStr"/>
       <c r="J355" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Chile']</t>
+          <t>['Chile', 'Switzerland']</t>
         </is>
       </c>
       <c r="K355" t="inlineStr">
@@ -30711,7 +30711,7 @@
       <c r="I356" t="inlineStr"/>
       <c r="J356" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Chile']</t>
+          <t>['Chile', 'Switzerland']</t>
         </is>
       </c>
       <c r="K356" t="inlineStr">
@@ -32601,7 +32601,7 @@
       <c r="I378" t="inlineStr"/>
       <c r="J378" t="inlineStr">
         <is>
-          <t>['Colombia', 'Ivory Coast']</t>
+          <t>['Ivory Coast', 'Colombia']</t>
         </is>
       </c>
       <c r="K378" t="inlineStr">
@@ -32685,7 +32685,7 @@
       </c>
       <c r="J379" t="inlineStr">
         <is>
-          <t>['Colombia', 'Ivory Coast']</t>
+          <t>['Ivory Coast', 'Colombia']</t>
         </is>
       </c>
       <c r="K379" t="inlineStr">
@@ -32773,7 +32773,7 @@
       </c>
       <c r="J380" t="inlineStr">
         <is>
-          <t>['Greece', 'Colombia']</t>
+          <t>['Colombia', 'Greece']</t>
         </is>
       </c>
       <c r="K380" t="inlineStr">
@@ -32861,7 +32861,7 @@
       </c>
       <c r="J381" t="inlineStr">
         <is>
-          <t>['Greece', 'Colombia']</t>
+          <t>['Ivory Coast', 'Colombia']</t>
         </is>
       </c>
       <c r="K381" t="inlineStr">
@@ -32871,34 +32871,38 @@
       </c>
       <c r="L381" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Ivory Coast</t>
         </is>
       </c>
       <c r="M381" t="inlineStr">
         <is>
+          <t>Japan</t>
+        </is>
+      </c>
+      <c r="N381" t="n">
+        <v>2</v>
+      </c>
+      <c r="O381" t="n">
+        <v>1</v>
+      </c>
+      <c r="P381" t="inlineStr">
+        <is>
           <t>Ivory Coast</t>
         </is>
       </c>
-      <c r="N381" t="n">
-        <v>1</v>
-      </c>
-      <c r="O381" t="n">
-        <v>-1</v>
-      </c>
-      <c r="P381" t="inlineStr"/>
       <c r="Q381" t="n">
         <v>0</v>
       </c>
       <c r="R381" t="inlineStr">
         <is>
-          <t>['Colombia', 'Greece']</t>
+          <t>['Colombia', 'Ivory Coast']</t>
         </is>
       </c>
       <c r="S381" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T381" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U381" t="n">
         <v>1785</v>
@@ -32949,7 +32953,7 @@
       </c>
       <c r="J382" t="inlineStr">
         <is>
-          <t>['Greece', 'Colombia']</t>
+          <t>['Ivory Coast', 'Colombia']</t>
         </is>
       </c>
       <c r="K382" t="inlineStr">
@@ -32959,19 +32963,19 @@
       </c>
       <c r="L382" t="inlineStr">
         <is>
+          <t>Ivory Coast</t>
+        </is>
+      </c>
+      <c r="M382" t="inlineStr">
+        <is>
           <t>Greece</t>
         </is>
       </c>
-      <c r="M382" t="inlineStr">
-        <is>
-          <t>Ivory Coast</t>
-        </is>
-      </c>
       <c r="N382" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O382" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="P382" t="inlineStr"/>
       <c r="Q382" t="n">
@@ -32979,14 +32983,14 @@
       </c>
       <c r="R382" t="inlineStr">
         <is>
-          <t>['Colombia', 'Greece']</t>
+          <t>['Colombia', 'Ivory Coast']</t>
         </is>
       </c>
       <c r="S382" t="n">
         <v>0</v>
       </c>
       <c r="T382" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U382" t="n">
         <v>1785</v>
@@ -33037,7 +33041,7 @@
       </c>
       <c r="J383" t="inlineStr">
         <is>
-          <t>['Colombia', 'Ivory Coast']</t>
+          <t>['Ivory Coast', 'Colombia']</t>
         </is>
       </c>
       <c r="K383" t="inlineStr">
@@ -33071,7 +33075,7 @@
         </is>
       </c>
       <c r="S383" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T383" t="n">
         <v>2</v>
@@ -33125,7 +33129,7 @@
       </c>
       <c r="J384" t="inlineStr">
         <is>
-          <t>['Colombia', 'Ivory Coast']</t>
+          <t>['Ivory Coast', 'Colombia']</t>
         </is>
       </c>
       <c r="K384" t="inlineStr">
@@ -33213,7 +33217,7 @@
       </c>
       <c r="J385" t="inlineStr">
         <is>
-          <t>['Colombia', 'Ivory Coast']</t>
+          <t>['Ivory Coast', 'Colombia']</t>
         </is>
       </c>
       <c r="K385" t="inlineStr">
@@ -33301,7 +33305,7 @@
       </c>
       <c r="J386" t="inlineStr">
         <is>
-          <t>['Greece', 'Colombia']</t>
+          <t>['Colombia', 'Greece']</t>
         </is>
       </c>
       <c r="K386" t="inlineStr">
@@ -33701,7 +33705,7 @@
       <c r="I391" t="inlineStr"/>
       <c r="J391" t="inlineStr">
         <is>
-          <t>['Switzerland', 'France']</t>
+          <t>['France', 'Switzerland']</t>
         </is>
       </c>
       <c r="K391" t="inlineStr">
@@ -33781,7 +33785,7 @@
       <c r="I392" t="inlineStr"/>
       <c r="J392" t="inlineStr">
         <is>
-          <t>['Switzerland', 'France']</t>
+          <t>['France', 'Switzerland']</t>
         </is>
       </c>
       <c r="K392" t="inlineStr">
@@ -33865,7 +33869,7 @@
       <c r="I393" t="inlineStr"/>
       <c r="J393" t="inlineStr">
         <is>
-          <t>['Switzerland', 'France']</t>
+          <t>['France', 'Switzerland']</t>
         </is>
       </c>
       <c r="K393" t="inlineStr">
@@ -33884,12 +33888,16 @@
         </is>
       </c>
       <c r="N393" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O393" t="n">
-        <v>-2</v>
-      </c>
-      <c r="P393" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="P393" t="inlineStr">
+        <is>
+          <t>Switzerland</t>
+        </is>
+      </c>
       <c r="Q393" t="n">
         <v>0</v>
       </c>
@@ -33953,7 +33961,7 @@
       </c>
       <c r="J394" t="inlineStr">
         <is>
-          <t>['Switzerland', 'France']</t>
+          <t>['France', 'Switzerland']</t>
         </is>
       </c>
       <c r="K394" t="inlineStr">
@@ -34045,7 +34053,7 @@
       </c>
       <c r="J395" t="inlineStr">
         <is>
-          <t>['Switzerland', 'France']</t>
+          <t>['France', 'Switzerland']</t>
         </is>
       </c>
       <c r="K395" t="inlineStr">
@@ -34137,7 +34145,7 @@
       </c>
       <c r="J396" t="inlineStr">
         <is>
-          <t>['Switzerland', 'France']</t>
+          <t>['France', 'Switzerland']</t>
         </is>
       </c>
       <c r="K396" t="inlineStr">
@@ -34215,7 +34223,7 @@
       <c r="I397" t="inlineStr"/>
       <c r="J397" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K397" t="inlineStr">
@@ -34299,7 +34307,7 @@
       </c>
       <c r="J398" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K398" t="inlineStr">
@@ -34391,7 +34399,7 @@
       </c>
       <c r="J399" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K399" t="inlineStr">
@@ -34479,7 +34487,7 @@
       </c>
       <c r="J400" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K400" t="inlineStr">
@@ -34567,7 +34575,7 @@
       </c>
       <c r="J401" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K401" t="inlineStr">
@@ -34655,7 +34663,7 @@
       </c>
       <c r="J402" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K402" t="inlineStr">
@@ -34743,7 +34751,7 @@
       </c>
       <c r="J403" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K403" t="inlineStr">
@@ -34831,7 +34839,7 @@
       </c>
       <c r="J404" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K404" t="inlineStr">
@@ -34919,7 +34927,7 @@
       </c>
       <c r="J405" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K405" t="inlineStr">
@@ -35007,7 +35015,7 @@
       </c>
       <c r="J406" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="K406" t="inlineStr">
@@ -35081,7 +35089,7 @@
       <c r="I407" t="inlineStr"/>
       <c r="J407" t="inlineStr">
         <is>
-          <t>['United States', 'Germany']</t>
+          <t>['Germany', 'United States']</t>
         </is>
       </c>
       <c r="K407" t="inlineStr">
@@ -35161,7 +35169,7 @@
       <c r="I408" t="inlineStr"/>
       <c r="J408" t="inlineStr">
         <is>
-          <t>['United States', 'Germany']</t>
+          <t>['Germany', 'United States']</t>
         </is>
       </c>
       <c r="K408" t="inlineStr">
@@ -35249,7 +35257,7 @@
       </c>
       <c r="J409" t="inlineStr">
         <is>
-          <t>['United States', 'Germany']</t>
+          <t>['Germany', 'United States']</t>
         </is>
       </c>
       <c r="K409" t="inlineStr">
@@ -35337,7 +35345,7 @@
       </c>
       <c r="J410" t="inlineStr">
         <is>
-          <t>['United States', 'Germany']</t>
+          <t>['Germany', 'United States']</t>
         </is>
       </c>
       <c r="K410" t="inlineStr">
@@ -35425,7 +35433,7 @@
       </c>
       <c r="J411" t="inlineStr">
         <is>
-          <t>['United States', 'Germany']</t>
+          <t>['Germany', 'United States']</t>
         </is>
       </c>
       <c r="K411" t="inlineStr">
@@ -35517,7 +35525,7 @@
       </c>
       <c r="J412" t="inlineStr">
         <is>
-          <t>['United States', 'Germany']</t>
+          <t>['Germany', 'United States']</t>
         </is>
       </c>
       <c r="K412" t="inlineStr">
@@ -35591,7 +35599,7 @@
       <c r="I413" t="inlineStr"/>
       <c r="J413" t="inlineStr">
         <is>
-          <t>['Belgium', 'Algeria']</t>
+          <t>['Algeria', 'Belgium']</t>
         </is>
       </c>
       <c r="K413" t="inlineStr">
@@ -35671,7 +35679,7 @@
       <c r="I414" t="inlineStr"/>
       <c r="J414" t="inlineStr">
         <is>
-          <t>['Belgium', 'Algeria']</t>
+          <t>['Algeria', 'Belgium']</t>
         </is>
       </c>
       <c r="K414" t="inlineStr">
@@ -35847,7 +35855,7 @@
       </c>
       <c r="J416" t="inlineStr">
         <is>
-          <t>['Belgium', 'Algeria']</t>
+          <t>['Algeria', 'Belgium']</t>
         </is>
       </c>
       <c r="K416" t="inlineStr">
@@ -35935,7 +35943,7 @@
       </c>
       <c r="J417" t="inlineStr">
         <is>
-          <t>['Belgium', 'Algeria']</t>
+          <t>['Algeria', 'Belgium']</t>
         </is>
       </c>
       <c r="K417" t="inlineStr">
@@ -38301,7 +38309,7 @@
       <c r="I445" t="inlineStr"/>
       <c r="J445" t="inlineStr">
         <is>
-          <t>['Brazil', 'Switzerland']</t>
+          <t>['Switzerland', 'Brazil']</t>
         </is>
       </c>
       <c r="K445" t="inlineStr">
@@ -38381,7 +38389,7 @@
       <c r="I446" t="inlineStr"/>
       <c r="J446" t="inlineStr">
         <is>
-          <t>['Brazil', 'Switzerland']</t>
+          <t>['Switzerland', 'Brazil']</t>
         </is>
       </c>
       <c r="K446" t="inlineStr">
@@ -38469,7 +38477,7 @@
       </c>
       <c r="J447" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Brazil']</t>
+          <t>['Brazil', 'Switzerland']</t>
         </is>
       </c>
       <c r="K447" t="inlineStr">
@@ -38557,7 +38565,7 @@
       </c>
       <c r="J448" t="inlineStr">
         <is>
-          <t>['Brazil', 'Switzerland']</t>
+          <t>['Switzerland', 'Brazil']</t>
         </is>
       </c>
       <c r="K448" t="inlineStr">
@@ -38645,7 +38653,7 @@
       </c>
       <c r="J449" t="inlineStr">
         <is>
-          <t>['Brazil', 'Switzerland']</t>
+          <t>['Switzerland', 'Brazil']</t>
         </is>
       </c>
       <c r="K449" t="inlineStr">
@@ -38733,7 +38741,7 @@
       </c>
       <c r="J450" t="inlineStr">
         <is>
-          <t>['Brazil', 'Switzerland']</t>
+          <t>['Switzerland', 'Brazil']</t>
         </is>
       </c>
       <c r="K450" t="inlineStr">
@@ -38821,7 +38829,7 @@
       </c>
       <c r="J451" t="inlineStr">
         <is>
-          <t>['Brazil', 'Switzerland']</t>
+          <t>['Switzerland', 'Brazil']</t>
         </is>
       </c>
       <c r="K451" t="inlineStr">
@@ -38909,7 +38917,7 @@
       </c>
       <c r="J452" t="inlineStr">
         <is>
-          <t>['Brazil', 'Switzerland']</t>
+          <t>['Switzerland', 'Brazil']</t>
         </is>
       </c>
       <c r="K452" t="inlineStr">
@@ -38983,7 +38991,7 @@
       <c r="I453" t="inlineStr"/>
       <c r="J453" t="inlineStr">
         <is>
-          <t>['Mexico', 'Germany']</t>
+          <t>['Germany', 'Mexico']</t>
         </is>
       </c>
       <c r="K453" t="inlineStr">
@@ -39063,7 +39071,7 @@
       <c r="I454" t="inlineStr"/>
       <c r="J454" t="inlineStr">
         <is>
-          <t>['Mexico', 'Germany']</t>
+          <t>['Germany', 'Mexico']</t>
         </is>
       </c>
       <c r="K454" t="inlineStr">
@@ -39147,7 +39155,7 @@
       <c r="I455" t="inlineStr"/>
       <c r="J455" t="inlineStr">
         <is>
-          <t>['Mexico', 'Germany']</t>
+          <t>['Germany', 'Mexico']</t>
         </is>
       </c>
       <c r="K455" t="inlineStr">
@@ -39235,7 +39243,7 @@
       </c>
       <c r="J456" t="inlineStr">
         <is>
-          <t>['Sweden', 'Mexico']</t>
+          <t>['Mexico', 'Sweden']</t>
         </is>
       </c>
       <c r="K456" t="inlineStr">
@@ -39327,7 +39335,7 @@
       </c>
       <c r="J457" t="inlineStr">
         <is>
-          <t>['Sweden', 'Mexico']</t>
+          <t>['Mexico', 'Sweden']</t>
         </is>
       </c>
       <c r="K457" t="inlineStr">
@@ -39419,7 +39427,7 @@
       </c>
       <c r="J458" t="inlineStr">
         <is>
-          <t>['Sweden', 'Mexico']</t>
+          <t>['Mexico', 'Sweden']</t>
         </is>
       </c>
       <c r="K458" t="inlineStr">
@@ -39511,7 +39519,7 @@
       </c>
       <c r="J459" t="inlineStr">
         <is>
-          <t>['Sweden', 'Mexico']</t>
+          <t>['Mexico', 'Sweden']</t>
         </is>
       </c>
       <c r="K459" t="inlineStr">
@@ -39599,7 +39607,7 @@
       </c>
       <c r="J460" t="inlineStr">
         <is>
-          <t>['Sweden', 'Mexico']</t>
+          <t>['Mexico', 'Sweden']</t>
         </is>
       </c>
       <c r="K460" t="inlineStr">
@@ -40179,7 +40187,7 @@
       <c r="I467" t="inlineStr"/>
       <c r="J467" t="inlineStr">
         <is>
-          <t>['Japan', 'Senegal']</t>
+          <t>['Senegal', 'Japan']</t>
         </is>
       </c>
       <c r="K467" t="inlineStr">
@@ -40259,7 +40267,7 @@
       <c r="I468" t="inlineStr"/>
       <c r="J468" t="inlineStr">
         <is>
-          <t>['Japan', 'Senegal']</t>
+          <t>['Senegal', 'Japan']</t>
         </is>
       </c>
       <c r="K468" t="inlineStr">
@@ -40343,7 +40351,7 @@
       <c r="I469" t="inlineStr"/>
       <c r="J469" t="inlineStr">
         <is>
-          <t>['Japan', 'Senegal']</t>
+          <t>['Senegal', 'Japan']</t>
         </is>
       </c>
       <c r="K469" t="inlineStr">
@@ -40431,7 +40439,7 @@
       </c>
       <c r="J470" t="inlineStr">
         <is>
-          <t>['Japan', 'Senegal']</t>
+          <t>['Senegal', 'Japan']</t>
         </is>
       </c>
       <c r="K470" t="inlineStr">
@@ -40519,7 +40527,7 @@
       </c>
       <c r="J471" t="inlineStr">
         <is>
-          <t>['Colombia', 'Senegal']</t>
+          <t>['Senegal', 'Colombia']</t>
         </is>
       </c>
       <c r="K471" t="inlineStr">
@@ -40593,7 +40601,7 @@
       <c r="I472" t="inlineStr"/>
       <c r="J472" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Ecuador']</t>
+          <t>['Ecuador', 'Netherlands']</t>
         </is>
       </c>
       <c r="K472" t="inlineStr">
@@ -40673,7 +40681,7 @@
       <c r="I473" t="inlineStr"/>
       <c r="J473" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Ecuador']</t>
+          <t>['Ecuador', 'Netherlands']</t>
         </is>
       </c>
       <c r="K473" t="inlineStr">
@@ -40761,7 +40769,7 @@
       </c>
       <c r="J474" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Ecuador']</t>
+          <t>['Ecuador', 'Netherlands']</t>
         </is>
       </c>
       <c r="K474" t="inlineStr">
@@ -41025,7 +41033,7 @@
       </c>
       <c r="J477" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Ecuador']</t>
+          <t>['Ecuador', 'Netherlands']</t>
         </is>
       </c>
       <c r="K477" t="inlineStr">
@@ -41187,7 +41195,7 @@
       <c r="I479" t="inlineStr"/>
       <c r="J479" t="inlineStr">
         <is>
-          <t>['England', 'Iran']</t>
+          <t>['Iran', 'England']</t>
         </is>
       </c>
       <c r="K479" t="inlineStr">
@@ -41267,7 +41275,7 @@
       <c r="I480" t="inlineStr"/>
       <c r="J480" t="inlineStr">
         <is>
-          <t>['England', 'Iran']</t>
+          <t>['Iran', 'England']</t>
         </is>
       </c>
       <c r="K480" t="inlineStr">
@@ -41351,7 +41359,7 @@
       <c r="I481" t="inlineStr"/>
       <c r="J481" t="inlineStr">
         <is>
-          <t>['England', 'Iran']</t>
+          <t>['Iran', 'England']</t>
         </is>
       </c>
       <c r="K481" t="inlineStr">
@@ -41439,7 +41447,7 @@
       </c>
       <c r="J482" t="inlineStr">
         <is>
-          <t>['England', 'United States']</t>
+          <t>['United States', 'England']</t>
         </is>
       </c>
       <c r="K482" t="inlineStr">
@@ -41527,7 +41535,7 @@
       </c>
       <c r="J483" t="inlineStr">
         <is>
-          <t>['England', 'United States']</t>
+          <t>['United States', 'England']</t>
         </is>
       </c>
       <c r="K483" t="inlineStr">
@@ -41615,7 +41623,7 @@
       </c>
       <c r="J484" t="inlineStr">
         <is>
-          <t>['England', 'United States']</t>
+          <t>['United States', 'England']</t>
         </is>
       </c>
       <c r="K484" t="inlineStr">
@@ -41703,7 +41711,7 @@
       </c>
       <c r="J485" t="inlineStr">
         <is>
-          <t>['England', 'United States']</t>
+          <t>['United States', 'England']</t>
         </is>
       </c>
       <c r="K485" t="inlineStr">
@@ -41777,7 +41785,7 @@
       <c r="I486" t="inlineStr"/>
       <c r="J486" t="inlineStr">
         <is>
-          <t>['Saudi Arabia', 'Poland']</t>
+          <t>['Poland', 'Saudi Arabia']</t>
         </is>
       </c>
       <c r="K486" t="inlineStr">
@@ -41857,7 +41865,7 @@
       <c r="I487" t="inlineStr"/>
       <c r="J487" t="inlineStr">
         <is>
-          <t>['Saudi Arabia', 'Poland']</t>
+          <t>['Poland', 'Saudi Arabia']</t>
         </is>
       </c>
       <c r="K487" t="inlineStr">
@@ -42371,7 +42379,7 @@
       <c r="I493" t="inlineStr"/>
       <c r="J493" t="inlineStr">
         <is>
-          <t>['Australia', 'France']</t>
+          <t>['France', 'Australia']</t>
         </is>
       </c>
       <c r="K493" t="inlineStr">
@@ -42451,7 +42459,7 @@
       <c r="I494" t="inlineStr"/>
       <c r="J494" t="inlineStr">
         <is>
-          <t>['Australia', 'France']</t>
+          <t>['France', 'Australia']</t>
         </is>
       </c>
       <c r="K494" t="inlineStr">
@@ -42539,7 +42547,7 @@
       <c r="I495" t="inlineStr"/>
       <c r="J495" t="inlineStr">
         <is>
-          <t>['Australia', 'France']</t>
+          <t>['France', 'Australia']</t>
         </is>
       </c>
       <c r="K495" t="inlineStr">
@@ -42631,7 +42639,7 @@
       </c>
       <c r="J496" t="inlineStr">
         <is>
-          <t>['Australia', 'France']</t>
+          <t>['France', 'Australia']</t>
         </is>
       </c>
       <c r="K496" t="inlineStr">
@@ -42719,7 +42727,7 @@
       </c>
       <c r="J497" t="inlineStr">
         <is>
-          <t>['Australia', 'France']</t>
+          <t>['France', 'Australia']</t>
         </is>
       </c>
       <c r="K497" t="inlineStr">
@@ -42793,7 +42801,7 @@
       <c r="I498" t="inlineStr"/>
       <c r="J498" t="inlineStr">
         <is>
-          <t>['Costa Rica', 'Spain']</t>
+          <t>['Spain', 'Costa Rica']</t>
         </is>
       </c>
       <c r="K498" t="inlineStr">
@@ -44073,7 +44081,7 @@
       <c r="I513" t="inlineStr"/>
       <c r="J513" t="inlineStr">
         <is>
-          <t>['Brazil', 'Switzerland']</t>
+          <t>['Switzerland', 'Brazil']</t>
         </is>
       </c>
       <c r="K513" t="inlineStr">
@@ -44153,7 +44161,7 @@
       <c r="I514" t="inlineStr"/>
       <c r="J514" t="inlineStr">
         <is>
-          <t>['Brazil', 'Switzerland']</t>
+          <t>['Switzerland', 'Brazil']</t>
         </is>
       </c>
       <c r="K514" t="inlineStr">
@@ -44245,7 +44253,7 @@
       </c>
       <c r="J515" t="inlineStr">
         <is>
-          <t>['Brazil', 'Switzerland']</t>
+          <t>['Switzerland', 'Brazil']</t>
         </is>
       </c>
       <c r="K515" t="inlineStr">
@@ -44333,7 +44341,7 @@
       </c>
       <c r="J516" t="inlineStr">
         <is>
-          <t>['Brazil', 'Switzerland']</t>
+          <t>['Switzerland', 'Brazil']</t>
         </is>
       </c>
       <c r="K516" t="inlineStr">
@@ -44425,7 +44433,7 @@
       </c>
       <c r="J517" t="inlineStr">
         <is>
-          <t>['Brazil', 'Serbia']</t>
+          <t>['Serbia', 'Brazil']</t>
         </is>
       </c>
       <c r="K517" t="inlineStr">
@@ -44513,7 +44521,7 @@
       </c>
       <c r="J518" t="inlineStr">
         <is>
-          <t>['Brazil', 'Switzerland']</t>
+          <t>['Switzerland', 'Brazil']</t>
         </is>
       </c>
       <c r="K518" t="inlineStr">
@@ -44605,7 +44613,7 @@
       </c>
       <c r="J519" t="inlineStr">
         <is>
-          <t>['Brazil', 'Switzerland']</t>
+          <t>['Switzerland', 'Brazil']</t>
         </is>
       </c>
       <c r="K519" t="inlineStr">
@@ -44693,7 +44701,7 @@
       </c>
       <c r="J520" t="inlineStr">
         <is>
-          <t>['Brazil', 'Switzerland']</t>
+          <t>['Switzerland', 'Brazil']</t>
         </is>
       </c>
       <c r="K520" t="inlineStr">
@@ -45027,7 +45035,7 @@
       </c>
       <c r="J524" t="inlineStr">
         <is>
-          <t>['Uruguay', 'Portugal']</t>
+          <t>['Portugal', 'Uruguay']</t>
         </is>
       </c>
       <c r="K524" t="inlineStr">
@@ -45115,7 +45123,7 @@
       </c>
       <c r="J525" t="inlineStr">
         <is>
-          <t>['Uruguay', 'Portugal']</t>
+          <t>['Portugal', 'Uruguay']</t>
         </is>
       </c>
       <c r="K525" t="inlineStr">
@@ -45203,7 +45211,7 @@
       </c>
       <c r="J526" t="inlineStr">
         <is>
-          <t>['Uruguay', 'Portugal']</t>
+          <t>['Portugal', 'Uruguay']</t>
         </is>
       </c>
       <c r="K526" t="inlineStr">

</xml_diff>